<commit_message>
balanced number of samples per features added
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t xml:space="preserve">method</t>
   </si>
@@ -43,76 +43,100 @@
     <t xml:space="preserve">scaled features</t>
   </si>
   <si>
+    <t xml:space="preserve">number of features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">white matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grey matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hippocampus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amygdala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thalamus</t>
+  </si>
+  <si>
     <t xml:space="preserve">evaluation results</t>
   </si>
   <si>
-    <t xml:space="preserve">white matter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grey matter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hippocampus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amygdala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thalamus</t>
-  </si>
-  <si>
     <t xml:space="preserve">importance of features</t>
   </si>
   <si>
-    <t xml:space="preserve">background</t>
-  </si>
-  <si>
     <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'z', 'T2 grad', 'y', 'x', 'T1 grad']</t>
   </si>
   <si>
     <t xml:space="preserve">['T2 intensity', 'z', 'y', 'T1 grad', 'T2 grad', 'T1 intensity', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">['T2 intensity', 'z', 'T1 grad', 'y', 'T2 grad', 'T1 intensity', 'x']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['T2 intensity', 'T1 intensity', 'T2 grad', 'T1 grad', 'y', 'z', 'x']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'z', 'T1 grad', 'T2 grad', 'x', 'y']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'T1 grad', 'T2 grad', 'z', 'y', 'x']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">svm_lin_ex1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">svm_lin_ex2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">position is not an important feature → bad segmentation of small structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balanced number of samples per class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ground truth is well aligned, should take position as important features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logistic regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LogisticRegression(C=10000, class_weight=None, dual=False, fit_intercept=True,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C = 10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          intercept_scaling=1, max_iter=100, multi_class='ovr', n_jobs=1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class_weights = None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          penalty='l2', random_state=None, solver='liblinear', tol=0.0001,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          verbose=0, warm_start=False)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fit_intercept = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">penalty = l2</t>
+  </si>
+  <si>
     <t xml:space="preserve">greay matter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['T2 intensity', 'z', 'T1 grad', 'y', 'T2 grad', 'T1 intensity', 'x']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['T2 intensity', 'T1 intensity', 'T2 grad', 'T1 grad', 'y', 'z', 'x']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'z', 'T1 grad', 'T2 grad', 'x', 'y']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'T1 grad', 'T2 grad', 'z', 'y', 'x']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logistic regression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LogisticRegression(C=10000, class_weight=None, dual=False, fit_intercept=True,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C = 10000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          intercept_scaling=1, max_iter=100, multi_class='ovr', n_jobs=1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class_weights = None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          penalty='l2', random_state=None, solver='liblinear', tol=0.0001,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          verbose=0, warm_start=False)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fit_intercept = True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">penalty = l2</t>
   </si>
   <si>
     <t xml:space="preserve">coordinates x</t>
@@ -369,271 +393,376 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:J58"/>
+  <dimension ref="A3:K64"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J5" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="J7" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="1" t="n">
-        <v>101915</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>103111</v>
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>127875</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>127875</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="B9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>0.78405</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>0.077738</v>
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>134450</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>134450</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>0.57433</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>0.60497</v>
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>106369</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>106369</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>0.01751</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>0.01872</v>
+        <v>11</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>25296</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>189930</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>0.02351</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>0.03161</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>8584</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>172295</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>26394</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1057278</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>15</v>
+      <c r="C14" s="1" t="n">
+        <v>101915</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>103111</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>101915</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>103111</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>16</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0.78405</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0.77738</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>18</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0.57433</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>0.60497</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>19</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0.01751</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0.01872</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>20</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0.02351</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>0.03161</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="I25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
+      <c r="D33" s="2"/>
+      <c r="E33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="n">
-        <v>101915</v>
-      </c>
-      <c r="D33" s="1" t="n">
-        <v>103111</v>
-      </c>
-      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -642,18 +771,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <v>0.78333</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>0.78865</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -662,16 +789,14 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <v>0.65864</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>0.62634</v>
-      </c>
-      <c r="E35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -680,16 +805,14 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>0.0038</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <v>0.00375</v>
-      </c>
-      <c r="E36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -698,15 +821,11 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1"/>
-      <c r="B37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -716,15 +835,11 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
-      <c r="B38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -733,14 +848,14 @@
       <c r="J38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="n">
+        <v>101915</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>103111</v>
+      </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -749,12 +864,18 @@
       <c r="J39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>0.78333</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>0.78865</v>
+      </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -765,10 +886,14 @@
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>0.65864</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>0.62634</v>
+      </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -779,10 +904,14 @@
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>0.0038</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>0.00375</v>
+      </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -793,10 +922,14 @@
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -807,10 +940,14 @@
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -819,9 +956,11 @@
       <c r="J44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B45" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -834,9 +973,11 @@
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -844,97 +985,95 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="3" t="s">
-        <v>39</v>
-      </c>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="B48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="B49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="B50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="B51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1"/>
+    <row r="53" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="B53" s="1"/>
       <c r="C53" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -948,7 +1087,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -962,7 +1101,7 @@
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -976,7 +1115,7 @@
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -990,7 +1129,7 @@
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -1004,7 +1143,7 @@
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -1013,6 +1152,90 @@
       <c r="H58" s="3"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added results for rbf
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="58">
   <si>
     <t xml:space="preserve">method</t>
   </si>
   <si>
     <t xml:space="preserve">SVM linear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVM rbf</t>
   </si>
   <si>
     <t xml:space="preserve">parameters</t>
@@ -323,7 +326,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -358,10 +361,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -443,19 +442,18 @@
   </sheetPr>
   <dimension ref="A3:Y52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S20" activeCellId="0" sqref="S20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y19" activeCellId="0" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>0</v>
       </c>
@@ -468,186 +466,225 @@
       <c r="Q3" s="0" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="X3" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>127875</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J8" s="1" t="n">
         <v>127875</v>
       </c>
       <c r="L8" s="1"/>
       <c r="Q8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R8" s="0" t="n">
         <v>127875</v>
       </c>
+      <c r="X8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>5826</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>134450</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J9" s="1" t="n">
         <v>134450</v>
       </c>
       <c r="L9" s="1"/>
       <c r="Q9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R9" s="0" t="n">
         <v>134450</v>
       </c>
+      <c r="X9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>6156</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>106369</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J10" s="1" t="n">
         <v>106369</v>
       </c>
       <c r="L10" s="1"/>
       <c r="Q10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R10" s="0" t="n">
         <v>106369</v>
       </c>
+      <c r="X10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>4865</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>25296</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J11" s="1" t="n">
         <v>189930</v>
       </c>
       <c r="L11" s="1"/>
       <c r="Q11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R11" s="0" t="n">
         <v>25296</v>
       </c>
+      <c r="X11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>4587</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>8584</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J12" s="1" t="n">
         <v>172295</v>
       </c>
       <c r="L12" s="1"/>
       <c r="Q12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R12" s="0" t="n">
         <v>8584</v>
       </c>
+      <c r="X12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <v>4806</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>26394</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J13" s="1" t="n">
         <v>132127</v>
       </c>
       <c r="L13" s="1"/>
       <c r="Q13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R13" s="0" t="n">
         <v>26394</v>
       </c>
+      <c r="X13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>6026</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>101915</v>
@@ -668,10 +705,13 @@
       <c r="S14" s="2" t="n">
         <v>103111</v>
       </c>
+      <c r="Y14" s="2" t="n">
+        <v>101915</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>0.78405</v>
@@ -680,7 +720,7 @@
         <v>0.77738</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J15" s="2" t="n">
         <v>0.76308</v>
@@ -690,7 +730,7 @@
       </c>
       <c r="L15" s="1"/>
       <c r="Q15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R15" s="2" t="n">
         <v>0.80922</v>
@@ -698,10 +738,16 @@
       <c r="S15" s="2" t="n">
         <v>0.80682</v>
       </c>
+      <c r="X15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y15" s="2" t="n">
+        <v>0.81542</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>0.57433</v>
@@ -710,7 +756,7 @@
         <v>0.60497</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J16" s="2" t="n">
         <v>0.4205</v>
@@ -720,7 +766,7 @@
       </c>
       <c r="L16" s="1"/>
       <c r="Q16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R16" s="2" t="n">
         <v>0.63349</v>
@@ -728,10 +774,16 @@
       <c r="S16" s="2" t="n">
         <v>0.66559</v>
       </c>
+      <c r="X16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="2" t="n">
+        <v>0.72717</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>0.01751</v>
@@ -740,7 +792,7 @@
         <v>0.01872</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J17" s="2" t="n">
         <v>0.02383</v>
@@ -750,7 +802,7 @@
       </c>
       <c r="L17" s="1"/>
       <c r="Q17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R17" s="2" t="n">
         <v>0.35124</v>
@@ -758,10 +810,16 @@
       <c r="S17" s="2" t="n">
         <v>0.39647</v>
       </c>
+      <c r="X17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y17" s="2" t="n">
+        <v>0.32313</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>0.02351</v>
@@ -770,7 +828,7 @@
         <v>0.03161</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J18" s="2" t="n">
         <v>0.02383</v>
@@ -780,7 +838,7 @@
       </c>
       <c r="L18" s="1"/>
       <c r="Q18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R18" s="2" t="n">
         <v>0.26467</v>
@@ -788,10 +846,16 @@
       <c r="S18" s="2" t="n">
         <v>0.31402</v>
       </c>
+      <c r="X18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y18" s="2" t="n">
+        <v>0.22086</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>0</v>
@@ -800,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J19" s="2" t="n">
         <v>0.05305</v>
@@ -810,7 +874,7 @@
       </c>
       <c r="L19" s="1"/>
       <c r="Q19" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R19" s="2" t="n">
         <v>0.64571</v>
@@ -818,102 +882,108 @@
       <c r="S19" s="2" t="n">
         <v>0.67325</v>
       </c>
+      <c r="X19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y19" s="2" t="n">
+        <v>0.49239</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -924,33 +994,33 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,7 +1029,7 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -969,7 +1039,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -979,7 +1049,7 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
@@ -1029,10 +1099,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>0.78343</v>
@@ -1046,7 +1116,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K35" s="2" t="n">
         <v>0.78338</v>
@@ -1060,7 +1130,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S35" s="2" t="n">
         <v>0.78529</v>
@@ -1077,7 +1147,7 @@
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>0.65866</v>
@@ -1091,7 +1161,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K36" s="2" t="n">
         <v>0.65865</v>
@@ -1105,7 +1175,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S36" s="2" t="n">
         <v>0.5929</v>
@@ -1122,7 +1192,7 @@
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>0.0038</v>
@@ -1136,7 +1206,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K37" s="2" t="n">
         <v>0.0038</v>
@@ -1150,7 +1220,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S37" s="2" t="n">
         <v>0.02457</v>
@@ -1167,7 +1237,7 @@
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>0</v>
@@ -1181,7 +1251,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K38" s="2" t="n">
         <v>0</v>
@@ -1195,7 +1265,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S38" s="2" t="n">
         <v>0.0329</v>
@@ -1212,7 +1282,7 @@
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>0</v>
@@ -1226,7 +1296,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K39" s="2" t="n">
         <v>0</v>
@@ -1240,7 +1310,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S39" s="2" t="n">
         <v>0.01239</v>
@@ -1256,13 +1326,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
@@ -1271,10 +1341,10 @@
       <c r="H40" s="5"/>
       <c r="I40" s="2"/>
       <c r="J40" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="5"/>
@@ -1283,10 +1353,10 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S40" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T40" s="4"/>
       <c r="U40" s="5"/>
@@ -1298,10 +1368,10 @@
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
       <c r="B41" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5"/>
@@ -1310,10 +1380,10 @@
       <c r="H41" s="5"/>
       <c r="I41" s="2"/>
       <c r="J41" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="5"/>
@@ -1322,10 +1392,10 @@
       <c r="P41" s="5"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S41" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T41" s="4"/>
       <c r="U41" s="5"/>
@@ -1337,10 +1407,10 @@
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
@@ -1349,10 +1419,10 @@
       <c r="H42" s="5"/>
       <c r="I42" s="2"/>
       <c r="J42" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="5"/>
@@ -1361,10 +1431,10 @@
       <c r="P42" s="5"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S42" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T42" s="4"/>
       <c r="U42" s="5"/>
@@ -1376,10 +1446,10 @@
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="5"/>
@@ -1388,10 +1458,10 @@
       <c r="H43" s="5"/>
       <c r="I43" s="2"/>
       <c r="J43" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L43" s="4"/>
       <c r="M43" s="5"/>
@@ -1400,10 +1470,10 @@
       <c r="P43" s="5"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S43" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T43" s="4"/>
       <c r="U43" s="5"/>
@@ -1415,10 +1485,10 @@
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="5"/>
@@ -1427,10 +1497,10 @@
       <c r="H44" s="5"/>
       <c r="I44" s="2"/>
       <c r="J44" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L44" s="4"/>
       <c r="M44" s="5"/>
@@ -1439,10 +1509,10 @@
       <c r="P44" s="5"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S44" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T44" s="4"/>
       <c r="U44" s="5"/>
@@ -1454,10 +1524,10 @@
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="5"/>
@@ -1466,10 +1536,10 @@
       <c r="H45" s="5"/>
       <c r="I45" s="2"/>
       <c r="J45" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="5"/>
@@ -1478,10 +1548,10 @@
       <c r="P45" s="5"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S45" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="T45" s="4"/>
       <c r="U45" s="5"/>
@@ -1519,10 +1589,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -1532,7 +1602,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -1542,7 +1612,7 @@
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
       <c r="R47" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
@@ -1554,61 +1624,51 @@
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
-      <c r="E49" s="9"/>
       <c r="J49" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R49" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
+      <c r="B50" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="J50" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R50" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
+      <c r="B51" s="0" t="s">
+        <v>54</v>
+      </c>
       <c r="J51" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R51" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
+      <c r="B52" s="0" t="s">
+        <v>56</v>
+      </c>
       <c r="J52" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R52" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
coordination feature importance added
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="66">
   <si>
     <t xml:space="preserve">method</t>
   </si>
@@ -109,30 +109,48 @@
     <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'T2 grad', 'z', 'x', 'T1 grad', 'y']</t>
   </si>
   <si>
+    <t xml:space="preserve">['xz', 'yz', 'y', 'z', 'x^2', 'z^2', 'y^2', 'xy', 'T2 intensity', 'T1 intensity', 'T2 grad', 'x', 'T1 grad']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T2 intensity', 'z', 'y', 'T1 grad', 'T2 grad', 'T1 intensity', 'x']</t>
   </si>
   <si>
     <t xml:space="preserve">['z', 'T2 intensity', 'y', 'T1 intensity', 'T2 grad', 'T1 grad', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">['yz', 'z^2', 'y', 'xz', 'z', 'xy', 'x^2', 'y^2', 'x', 'T2 intensity', 'T1 intensity', 'T2 grad', 'T1 grad']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T2 intensity', 'z', 'T1 grad', 'y', 'T2 grad', 'T1 intensity', 'x']</t>
   </si>
   <si>
     <t xml:space="preserve">['T2 intensity', 'z', 'y', 'T2 grad', 'x', 'T1 intensity', 'T1 grad']</t>
   </si>
   <si>
+    <t xml:space="preserve">['z^2', 'y', 'yz', 'z', 'xz', 'x^2', 'xy', 'y^2', 'x', 'T1 intensity', 'T2 intensity', 'T2 grad', 'T1 grad']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T2 intensity', 'T1 intensity', 'T2 grad', 'T1 grad', 'y', 'z', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">['T2 intensity', 'yz', 'xz', 'x^2', 'T2 grad', 'T1 intensity', 'T1 grad', 'z^2', 'y', 'z', 'xy', 'x', 'y^2']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'z', 'T1 grad', 'T2 grad', 'x', 'y']</t>
   </si>
   <si>
     <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'z', 'T2 grad', 'T1 grad', 'y', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">['T1 intensity', 'yz', 'xz', 'x^2', 'y', 'T2 intensity', 'T2 grad', 'z', 'xy', 'T1 grad', 'x', 'y^2', 'z^2']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'T1 grad', 'T2 grad', 'z', 'y', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'T1 grad', 'z', 'T2 grad', 'y', 'yz', 'z^2', 'x^2', 'x', 'xy', 'y^2', 'xz']</t>
+  </si>
+  <si>
     <t xml:space="preserve">results folder</t>
   </si>
   <si>
@@ -142,6 +160,9 @@
     <t xml:space="preserve">svm_lin_ex2</t>
   </si>
   <si>
+    <t xml:space="preserve">svm_lin_ex3</t>
+  </si>
+  <si>
     <t xml:space="preserve">comments</t>
   </si>
   <si>
@@ -151,7 +172,13 @@
     <t xml:space="preserve">balanced number of samples per class</t>
   </si>
   <si>
+    <t xml:space="preserve">second order features show tendency for ellipsoids in the segmentation</t>
+  </si>
+  <si>
     <t xml:space="preserve">ground truth is well aligned, should take position as important features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventricles should be segmented as background but are not → intensity should be good features</t>
   </si>
   <si>
     <t xml:space="preserve">logistic regression</t>
@@ -323,7 +350,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -358,10 +385,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -443,16 +466,15 @@
   </sheetPr>
   <dimension ref="A3:Y52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S20" activeCellId="0" sqref="S20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q30" activeCellId="0" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,7 +841,7 @@
         <v>0.67325</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>17</v>
       </c>
@@ -837,86 +859,122 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q21" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="R24" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
+      <c r="Q25" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K26" s="1"/>
@@ -924,33 +982,42 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
+      <c r="Q27" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
+      <c r="Q28" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
+      </c>
+      <c r="Q29" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,7 +1026,7 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -969,7 +1036,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -979,7 +1046,7 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
@@ -1077,7 +1144,7 @@
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>0.65866</v>
@@ -1091,7 +1158,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="K36" s="2" t="n">
         <v>0.65865</v>
@@ -1105,7 +1172,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="S36" s="2" t="n">
         <v>0.5929</v>
@@ -1262,7 +1329,7 @@
         <v>10</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
@@ -1274,7 +1341,7 @@
         <v>10</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="5"/>
@@ -1286,7 +1353,7 @@
         <v>10</v>
       </c>
       <c r="S40" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="T40" s="4"/>
       <c r="U40" s="5"/>
@@ -1301,7 +1368,7 @@
         <v>11</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5"/>
@@ -1313,7 +1380,7 @@
         <v>11</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="5"/>
@@ -1325,7 +1392,7 @@
         <v>11</v>
       </c>
       <c r="S41" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="T41" s="4"/>
       <c r="U41" s="5"/>
@@ -1340,7 +1407,7 @@
         <v>12</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
@@ -1352,7 +1419,7 @@
         <v>12</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="5"/>
@@ -1364,7 +1431,7 @@
         <v>12</v>
       </c>
       <c r="S42" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="T42" s="4"/>
       <c r="U42" s="5"/>
@@ -1379,7 +1446,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="5"/>
@@ -1391,7 +1458,7 @@
         <v>13</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="L43" s="4"/>
       <c r="M43" s="5"/>
@@ -1403,7 +1470,7 @@
         <v>13</v>
       </c>
       <c r="S43" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="T43" s="4"/>
       <c r="U43" s="5"/>
@@ -1442,7 +1509,7 @@
         <v>14</v>
       </c>
       <c r="S44" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="T44" s="4"/>
       <c r="U44" s="5"/>
@@ -1457,7 +1524,7 @@
         <v>15</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="5"/>
@@ -1469,7 +1536,7 @@
         <v>15</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="5"/>
@@ -1481,7 +1548,7 @@
         <v>15</v>
       </c>
       <c r="S45" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="T45" s="4"/>
       <c r="U45" s="5"/>
@@ -1519,10 +1586,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -1532,7 +1599,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -1542,7 +1609,7 @@
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
       <c r="R47" s="6" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
@@ -1557,58 +1624,48 @@
         <v>2</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
-      <c r="E49" s="9"/>
       <c r="J49" s="0" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="R49" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
+      <c r="B50" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="J50" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R50" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
+      <c r="B51" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="J51" s="0" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="R51" s="0" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
+      <c r="B52" s="0" t="s">
+        <v>64</v>
+      </c>
       <c r="J52" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="R52" s="0" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added possibility to have second order poylnomial coordination features
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="67">
   <si>
     <t xml:space="preserve">method</t>
   </si>
@@ -112,30 +112,48 @@
     <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'T2 grad', 'z', 'x', 'T1 grad', 'y']</t>
   </si>
   <si>
+    <t xml:space="preserve">['xz', 'yz', 'y', 'z', 'x^2', 'z^2', 'y^2', 'xy', 'T2 intensity', 'T1 intensity', 'T2 grad', 'x', 'T1 grad']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T2 intensity', 'z', 'y', 'T1 grad', 'T2 grad', 'T1 intensity', 'x']</t>
   </si>
   <si>
     <t xml:space="preserve">['z', 'T2 intensity', 'y', 'T1 intensity', 'T2 grad', 'T1 grad', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">['yz', 'z^2', 'y', 'xz', 'z', 'xy', 'x^2', 'y^2', 'x', 'T2 intensity', 'T1 intensity', 'T2 grad', 'T1 grad']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T2 intensity', 'z', 'T1 grad', 'y', 'T2 grad', 'T1 intensity', 'x']</t>
   </si>
   <si>
     <t xml:space="preserve">['T2 intensity', 'z', 'y', 'T2 grad', 'x', 'T1 intensity', 'T1 grad']</t>
   </si>
   <si>
+    <t xml:space="preserve">['z^2', 'y', 'yz', 'z', 'xz', 'x^2', 'xy', 'y^2', 'x', 'T1 intensity', 'T2 intensity', 'T2 grad', 'T1 grad']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T2 intensity', 'T1 intensity', 'T2 grad', 'T1 grad', 'y', 'z', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">['T2 intensity', 'yz', 'xz', 'x^2', 'T2 grad', 'T1 intensity', 'T1 grad', 'z^2', 'y', 'z', 'xy', 'x', 'y^2']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'z', 'T1 grad', 'T2 grad', 'x', 'y']</t>
   </si>
   <si>
     <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'z', 'T2 grad', 'T1 grad', 'y', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">['T1 intensity', 'yz', 'xz', 'x^2', 'y', 'T2 intensity', 'T2 grad', 'z', 'xy', 'T1 grad', 'x', 'y^2', 'z^2']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'T1 grad', 'T2 grad', 'z', 'y', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">['T1 intensity', 'T2 intensity', 'T1 grad', 'z', 'T2 grad', 'y', 'yz', 'z^2', 'x^2', 'x', 'xy', 'y^2', 'xz']</t>
+  </si>
+  <si>
     <t xml:space="preserve">results folder</t>
   </si>
   <si>
@@ -145,6 +163,9 @@
     <t xml:space="preserve">svm_lin_ex2</t>
   </si>
   <si>
+    <t xml:space="preserve">svm_lin_ex3</t>
+  </si>
+  <si>
     <t xml:space="preserve">comments</t>
   </si>
   <si>
@@ -154,7 +175,13 @@
     <t xml:space="preserve">balanced number of samples per class</t>
   </si>
   <si>
+    <t xml:space="preserve">second order features show tendency for ellipsoids in the segmentation</t>
+  </si>
+  <si>
     <t xml:space="preserve">ground truth is well aligned, should take position as important features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventricles should be segmented as background but are not → intensity should be good features</t>
   </si>
   <si>
     <t xml:space="preserve">logistic regression</t>
@@ -442,15 +469,17 @@
   </sheetPr>
   <dimension ref="A3:Y52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y19" activeCellId="0" sqref="Y19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W13" activeCellId="0" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="40.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,7 +918,7 @@
         <v>0.49239</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>18</v>
       </c>
@@ -907,120 +936,165 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q20" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="R24" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q27" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q28" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="Q29" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,7 +1103,7 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -1039,7 +1113,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1049,7 +1123,7 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
@@ -1147,7 +1221,7 @@
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>0.65866</v>
@@ -1161,7 +1235,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="K36" s="2" t="n">
         <v>0.65865</v>
@@ -1175,7 +1249,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="S36" s="2" t="n">
         <v>0.5929</v>
@@ -1332,7 +1406,7 @@
         <v>11</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
@@ -1344,7 +1418,7 @@
         <v>11</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="5"/>
@@ -1356,7 +1430,7 @@
         <v>11</v>
       </c>
       <c r="S40" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="T40" s="4"/>
       <c r="U40" s="5"/>
@@ -1371,7 +1445,7 @@
         <v>12</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5"/>
@@ -1383,7 +1457,7 @@
         <v>12</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="5"/>
@@ -1395,7 +1469,7 @@
         <v>12</v>
       </c>
       <c r="S41" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="T41" s="4"/>
       <c r="U41" s="5"/>
@@ -1410,7 +1484,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
@@ -1422,7 +1496,7 @@
         <v>13</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="5"/>
@@ -1434,7 +1508,7 @@
         <v>13</v>
       </c>
       <c r="S42" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="T42" s="4"/>
       <c r="U42" s="5"/>
@@ -1449,7 +1523,7 @@
         <v>14</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="5"/>
@@ -1461,7 +1535,7 @@
         <v>14</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="L43" s="4"/>
       <c r="M43" s="5"/>
@@ -1473,7 +1547,7 @@
         <v>14</v>
       </c>
       <c r="S43" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="T43" s="4"/>
       <c r="U43" s="5"/>
@@ -1512,7 +1586,7 @@
         <v>15</v>
       </c>
       <c r="S44" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="T44" s="4"/>
       <c r="U44" s="5"/>
@@ -1527,7 +1601,7 @@
         <v>16</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="5"/>
@@ -1539,7 +1613,7 @@
         <v>16</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="5"/>
@@ -1551,7 +1625,7 @@
         <v>16</v>
       </c>
       <c r="S45" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="T45" s="4"/>
       <c r="U45" s="5"/>
@@ -1589,10 +1663,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -1602,7 +1676,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -1612,7 +1686,7 @@
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
       <c r="R47" s="6" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
@@ -1627,48 +1701,48 @@
         <v>3</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="J49" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="R49" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="R50" s="0" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="R51" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="R52" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results with larger dataset
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -500,16 +500,17 @@
   <dimension ref="A3:AO65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF24" activeCellId="0" sqref="AF24"/>
+      <selection pane="topLeft" activeCell="AK20" activeCellId="0" sqref="AK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="22" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,6 +1080,9 @@
       <c r="AJ15" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="AK15" s="0" t="n">
+        <v>0.83868</v>
+      </c>
       <c r="AN15" s="0" t="s">
         <v>20</v>
       </c>
@@ -1142,6 +1146,9 @@
       <c r="AJ16" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="AK16" s="0" t="n">
+        <v>0.75114</v>
+      </c>
       <c r="AN16" s="0" t="s">
         <v>21</v>
       </c>
@@ -1205,6 +1212,9 @@
       <c r="AJ17" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="AK17" s="0" t="n">
+        <v>0.64543</v>
+      </c>
       <c r="AN17" s="0" t="s">
         <v>22</v>
       </c>
@@ -1268,6 +1278,9 @@
       <c r="AJ18" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="AK18" s="0" t="n">
+        <v>0.62178</v>
+      </c>
       <c r="AN18" s="0" t="s">
         <v>23</v>
       </c>
@@ -1330,6 +1343,9 @@
       </c>
       <c r="AJ19" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="AK19" s="0" t="n">
+        <v>0.77582</v>
       </c>
       <c r="AN19" s="0" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
added Housedorf to pipeline_utilities
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="94">
   <si>
     <t xml:space="preserve">method</t>
   </si>
@@ -208,18 +208,57 @@
     <t xml:space="preserve">Ventricles should be segmented as background but are not → intensity should be good features</t>
   </si>
   <si>
+    <t xml:space="preserve">SVM rbf with different measures</t>
+  </si>
+  <si>
     <t xml:space="preserve">ground truth labels are well registered and position is a very good feature (tested with sum over all ground truth labels)</t>
   </si>
   <si>
     <t xml:space="preserve">Limitation of segmentation is probably due to low order poylnomials (→ only ellipses possible where we would need symmetric but seperated clusters)</t>
   </si>
   <si>
+    <t xml:space="preserve">C1, g0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPCFTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNSVTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDRFDST</t>
+  </si>
+  <si>
     <t xml:space="preserve">logistic regression</t>
   </si>
   <si>
+    <t xml:space="preserve">WhiteMatter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreyMatter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hippocampus</t>
+  </si>
+  <si>
     <t xml:space="preserve">greay matter</t>
   </si>
   <si>
+    <t xml:space="preserve">Amygdala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalamus</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T1 intensity', 'T2 grad', 'z', 'T2 intensity', 'T1 grad', 'x', 'y']</t>
   </si>
   <si>
@@ -235,6 +274,15 @@
     <t xml:space="preserve">['T2 intensity', 'z', 'T1 intensity', 'y', 'T1 grad', 'T2 grad', 'x']</t>
   </si>
   <si>
+    <t xml:space="preserve">c15, g5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduced set increased datapoints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datapoints used</t>
+  </si>
+  <si>
     <t xml:space="preserve">['T2 intensity', 'T1 intensity', 'T2 grad', 'y', 'T1 grad', 'z', 'x']</t>
   </si>
   <si>
@@ -278,6 +326,9 @@
   </si>
   <si>
     <t xml:space="preserve">          solver='liblinear', tol=0.0001, verbose=0, warm_start=False)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c15, g10</t>
   </si>
 </sst>
 </file>
@@ -497,20 +548,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:AO65536"/>
+  <dimension ref="A3:AV65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK20" activeCellId="0" sqref="AK20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AV49" activeCellId="0" sqref="AV49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="22" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="37.3928571428571"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,15 +1581,41 @@
       <c r="Q29" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="AG29" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q30" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q31" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="AG31" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG32" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH32" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI32" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ32" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK32" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL32" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,7 +1624,7 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -1559,7 +1634,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1569,7 +1644,7 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
@@ -1577,6 +1652,24 @@
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
+      <c r="AG33" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH33" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI33" s="0" t="n">
+        <v>0.813977023211321</v>
+      </c>
+      <c r="AJ33" s="0" t="n">
+        <v>0.972735175115291</v>
+      </c>
+      <c r="AK33" s="0" t="n">
+        <v>0.956173233197534</v>
+      </c>
+      <c r="AL33" s="0" t="n">
+        <v>16.3095064303001</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
@@ -1616,6 +1709,24 @@
       <c r="W34" s="2"/>
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
+      <c r="AG34" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH34" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI34" s="0" t="n">
+        <v>0.7221034486147</v>
+      </c>
+      <c r="AJ34" s="0" t="n">
+        <v>0.94256664135942</v>
+      </c>
+      <c r="AK34" s="0" t="n">
+        <v>0.965790382781228</v>
+      </c>
+      <c r="AL34" s="0" t="n">
+        <v>18.0277563773199</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
@@ -1663,11 +1774,29 @@
       <c r="W35" s="2"/>
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
+      <c r="AG35" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH35" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI35" s="0" t="n">
+        <v>0.371505649607069</v>
+      </c>
+      <c r="AJ35" s="0" t="n">
+        <v>0.995529510135054</v>
+      </c>
+      <c r="AK35" s="0" t="n">
+        <v>0.958345940494201</v>
+      </c>
+      <c r="AL35" s="0" t="n">
+        <v>36.2491379207837</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>0.65866</v>
@@ -1681,7 +1810,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="K36" s="2" t="n">
         <v>0.65865</v>
@@ -1695,7 +1824,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="S36" s="2" t="n">
         <v>0.5929</v>
@@ -1708,6 +1837,24 @@
       <c r="W36" s="2"/>
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
+      <c r="AG36" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH36" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI36" s="0" t="n">
+        <v>0.293909287257019</v>
+      </c>
+      <c r="AJ36" s="0" t="n">
+        <v>0.997716594230984</v>
+      </c>
+      <c r="AK36" s="0" t="n">
+        <v>0.965654271927335</v>
+      </c>
+      <c r="AL36" s="0" t="n">
+        <v>96.3431367560762</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
@@ -1753,6 +1900,24 @@
       <c r="W37" s="2"/>
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
+      <c r="AG37" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH37" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI37" s="0" t="n">
+        <v>0.540803469393735</v>
+      </c>
+      <c r="AJ37" s="0" t="n">
+        <v>0.995602297771913</v>
+      </c>
+      <c r="AK37" s="0" t="n">
+        <v>0.991405242801891</v>
+      </c>
+      <c r="AL37" s="0" t="n">
+        <v>22.6715680975093</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
@@ -1852,7 +2017,7 @@
         <v>19</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
@@ -1864,7 +2029,7 @@
         <v>19</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="5"/>
@@ -1876,7 +2041,7 @@
         <v>19</v>
       </c>
       <c r="S40" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="T40" s="4"/>
       <c r="U40" s="5"/>
@@ -1891,7 +2056,7 @@
         <v>20</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5"/>
@@ -1903,7 +2068,7 @@
         <v>20</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="5"/>
@@ -1915,7 +2080,7 @@
         <v>20</v>
       </c>
       <c r="S41" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="T41" s="4"/>
       <c r="U41" s="5"/>
@@ -1930,7 +2095,7 @@
         <v>21</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
@@ -1942,7 +2107,7 @@
         <v>21</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="5"/>
@@ -1954,7 +2119,7 @@
         <v>21</v>
       </c>
       <c r="S42" s="0" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="T42" s="4"/>
       <c r="U42" s="5"/>
@@ -1962,6 +2127,18 @@
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
       <c r="Y42" s="2"/>
+      <c r="AG42" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN42" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO42" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU42" s="0" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
@@ -1969,7 +2146,7 @@
         <v>22</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="5"/>
@@ -1981,7 +2158,7 @@
         <v>22</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="L43" s="4"/>
       <c r="M43" s="5"/>
@@ -1993,7 +2170,7 @@
         <v>22</v>
       </c>
       <c r="S43" s="0" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="T43" s="4"/>
       <c r="U43" s="5"/>
@@ -2001,6 +2178,48 @@
       <c r="W43" s="5"/>
       <c r="X43" s="5"/>
       <c r="Y43" s="2"/>
+      <c r="AG43" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH43" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI43" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ43" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK43" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL43" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN43" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO43" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP43" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ43" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR43" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS43" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU43" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV43" s="0" t="n">
+        <v>12706</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
@@ -2032,7 +2251,7 @@
         <v>23</v>
       </c>
       <c r="S44" s="0" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="T44" s="4"/>
       <c r="U44" s="5"/>
@@ -2040,6 +2259,48 @@
       <c r="W44" s="5"/>
       <c r="X44" s="5"/>
       <c r="Y44" s="2"/>
+      <c r="AG44" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH44" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI44" s="0" t="n">
+        <v>0.838680965736394</v>
+      </c>
+      <c r="AJ44" s="0" t="n">
+        <v>0.977096831109586</v>
+      </c>
+      <c r="AK44" s="0" t="n">
+        <v>0.9607222967022</v>
+      </c>
+      <c r="AL44" s="0" t="n">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="AN44" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AO44" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP44" s="0" t="n">
+        <v>0.8343252772</v>
+      </c>
+      <c r="AQ44" s="0" t="n">
+        <v>0.9762439639</v>
+      </c>
+      <c r="AR44" s="0" t="n">
+        <v>0.9609652605</v>
+      </c>
+      <c r="AS44" s="0" t="n">
+        <v>14.8660687473</v>
+      </c>
+      <c r="AU44" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="AV44" s="0" t="n">
+        <v>134244</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
@@ -2047,7 +2308,7 @@
         <v>24</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="5"/>
@@ -2059,7 +2320,7 @@
         <v>24</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="5"/>
@@ -2071,7 +2332,7 @@
         <v>24</v>
       </c>
       <c r="S45" s="0" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="T45" s="4"/>
       <c r="U45" s="5"/>
@@ -2079,6 +2340,48 @@
       <c r="W45" s="5"/>
       <c r="X45" s="5"/>
       <c r="Y45" s="2"/>
+      <c r="AG45" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH45" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI45" s="0" t="n">
+        <v>0.751142434818436</v>
+      </c>
+      <c r="AJ45" s="0" t="n">
+        <v>0.954703019489519</v>
+      </c>
+      <c r="AK45" s="0" t="n">
+        <v>0.937859068618248</v>
+      </c>
+      <c r="AL45" s="0" t="n">
+        <v>16.1554944214035</v>
+      </c>
+      <c r="AN45" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AO45" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP45" s="0" t="n">
+        <v>0.7537801704</v>
+      </c>
+      <c r="AQ45" s="0" t="n">
+        <v>0.9558866262</v>
+      </c>
+      <c r="AR45" s="0" t="n">
+        <v>0.9343049934</v>
+      </c>
+      <c r="AS45" s="0" t="n">
+        <v>16.9115345253</v>
+      </c>
+      <c r="AU45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="AV45" s="0" t="n">
+        <v>109600</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
@@ -2106,13 +2409,55 @@
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
+      <c r="AG46" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH46" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI46" s="0" t="n">
+        <v>0.645431568742859</v>
+      </c>
+      <c r="AJ46" s="0" t="n">
+        <v>0.998641118702866</v>
+      </c>
+      <c r="AK46" s="0" t="n">
+        <v>0.940090771558245</v>
+      </c>
+      <c r="AL46" s="0" t="n">
+        <v>19.7989898732233</v>
+      </c>
+      <c r="AN46" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AO46" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP46" s="0" t="n">
+        <v>0.6450764653</v>
+      </c>
+      <c r="AQ46" s="0" t="n">
+        <v>0.9986385832</v>
+      </c>
+      <c r="AR46" s="0" t="n">
+        <v>0.9401916288</v>
+      </c>
+      <c r="AS46" s="0" t="n">
+        <v>17.0880074906</v>
+      </c>
+      <c r="AU46" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV46" s="0" t="n">
+        <v>24925</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2122,7 +2467,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -2132,7 +2477,7 @@
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
       <c r="R47" s="6" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
@@ -2141,55 +2486,265 @@
       <c r="W47" s="6"/>
       <c r="X47" s="6"/>
       <c r="Y47" s="6"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="AG47" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH47" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI47" s="0" t="n">
+        <v>0.621780303030303</v>
+      </c>
+      <c r="AJ47" s="0" t="n">
+        <v>0.999471685346263</v>
+      </c>
+      <c r="AK47" s="0" t="n">
+        <v>0.931876241839342</v>
+      </c>
+      <c r="AL47" s="0" t="n">
+        <v>28.2311884269862</v>
+      </c>
+      <c r="AN47" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AO47" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP47" s="0" t="n">
+        <v>0.6311076504</v>
+      </c>
+      <c r="AQ47" s="0" t="n">
+        <v>0.9995061651</v>
+      </c>
+      <c r="AR47" s="0" t="n">
+        <v>0.9202384332</v>
+      </c>
+      <c r="AS47" s="0" t="n">
+        <v>24.7386337537</v>
+      </c>
+      <c r="AU47" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AV47" s="0" t="n">
+        <v>8278</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG48" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH48" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI48" s="0" t="n">
+        <v>0.77581553501222</v>
+      </c>
+      <c r="AJ48" s="0" t="n">
+        <v>0.998563434196161</v>
+      </c>
+      <c r="AK48" s="0" t="n">
+        <v>0.98050064460679</v>
+      </c>
+      <c r="AL48" s="0" t="n">
+        <v>11.916375287813</v>
+      </c>
+      <c r="AN48" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AO48" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP48" s="0" t="n">
+        <v>0.7663076568</v>
+      </c>
+      <c r="AQ48" s="0" t="n">
+        <v>0.9984817759</v>
+      </c>
+      <c r="AR48" s="0" t="n">
+        <v>0.9803394929</v>
+      </c>
+      <c r="AS48" s="0" t="n">
+        <v>16.0623784042</v>
+      </c>
+      <c r="AU48" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AV48" s="0" t="n">
+        <v>27100</v>
+      </c>
+    </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>4</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="J49" s="0" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="R49" s="0" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="R50" s="0" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="R51" s="0" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="R52" s="0" t="s">
-        <v>76</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG53" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG54" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH54" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI54" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ54" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK54" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL54" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG55" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH55" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI55" s="0" t="n">
+        <v>0.839441540791141</v>
+      </c>
+      <c r="AJ55" s="0" t="n">
+        <v>0.978206310525178</v>
+      </c>
+      <c r="AK55" s="0" t="n">
+        <v>0.950650145127491</v>
+      </c>
+      <c r="AL55" s="0" t="n">
+        <v>12.0830459735946</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG56" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH56" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI56" s="0" t="n">
+        <v>0.615801031737063</v>
+      </c>
+      <c r="AJ56" s="0" t="n">
+        <v>0.908709924976914</v>
+      </c>
+      <c r="AK56" s="0" t="n">
+        <v>0.946339659199291</v>
+      </c>
+      <c r="AL56" s="0" t="n">
+        <v>23.1084400165827</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG57" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH57" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI57" s="0" t="n">
+        <v>0.67814164896986</v>
+      </c>
+      <c r="AJ57" s="0" t="n">
+        <v>0.998897766543996</v>
+      </c>
+      <c r="AK57" s="0" t="n">
+        <v>0.917902168431669</v>
+      </c>
+      <c r="AL57" s="0" t="n">
+        <v>10.6301458127347</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG58" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH58" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI58" s="0" t="n">
+        <v>0.657816198415149</v>
+      </c>
+      <c r="AJ58" s="0" t="n">
+        <v>0.999578080092726</v>
+      </c>
+      <c r="AK58" s="0" t="n">
+        <v>0.907181379506103</v>
+      </c>
+      <c r="AL58" s="0" t="n">
+        <v>27.8567765543682</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG59" s="0" t="n">
+        <v>101915</v>
+      </c>
+      <c r="AH59" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI59" s="0" t="n">
+        <v>0.80152433588875</v>
+      </c>
+      <c r="AJ59" s="0" t="n">
+        <v>0.998833231013631</v>
+      </c>
+      <c r="AK59" s="0" t="n">
+        <v>0.965996991834981</v>
+      </c>
+      <c r="AL59" s="0" t="n">
+        <v>10.0498756211209</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>